<commit_message>
Some galician songs have been changed.
</commit_message>
<xml_diff>
--- a/ids.xlsx
+++ b/ids.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\hilda\folkdataset\folkdataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603FD61B-6B51-4096-8C23-C805E3645749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC37A5F-C03A-4B6E-91F5-0FA53455F974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2115" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1009,15 +1009,9 @@
     <t>pezas_alalas_canta-o-merlo-na-silveira_canta-o-merlo-na-silveira-partitura_1_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_alalas_de-manancina_de-manancina-partitura_1_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_foliadas_a-feira-de-paiosaco_a-feira-de-paiosaco-partitura_2_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_foliadas_a-rianxeira_a-rianxeira-partitura_2_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_foliadas_amor-rianxeiro_amor-rianxeiro-partitura_2_e_1.krn</t>
   </si>
   <si>
@@ -1051,9 +1045,6 @@
     <t>pezas_foliadas_foliada-de-berducido_foliada-de-berducido-partitura-2_1_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_foliadas_foliada-de-berducido_foliada-de-berducido-partitura_1_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_foliadas_foliada-de-bora_foliada-de-bora-partitura_1_e_1.krn</t>
   </si>
   <si>
@@ -1063,9 +1054,6 @@
     <t>pezas_foliadas_foliada-de-carril_foliada-de-carril-partitura_2_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_foliadas_foliada-de-combarro_foliada-de-combarro-partitura_1_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_foliadas_foliada-de-conxo_foliada-de-conxo-partitura_1_e_1.krn</t>
   </si>
   <si>
@@ -1084,9 +1072,6 @@
     <t>pezas_foliadas_foliada-de-san-tirso_foliada-de-san-tirso-partitura-1_1_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_foliadas_foliada-de-vilaboa_foliada-de-vilaboa-partitura-1_2_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_foliadas_foliada-de-vilaboa_foliada-de-vilaboa-partitura_1_e_1.krn</t>
   </si>
   <si>
@@ -1108,9 +1093,6 @@
     <t>pezas_jotas_a-regueifa_a-regueifa-partitura_2_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_jotas_aforamento-dunha-jota-de-auga-nun-micromatraz_aforamento-dunha-jota-de-auga-nun-micromatraz-partitura_1_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_jotas_alghun-dia_alghun-dia-partitura_1_e_1.krn</t>
   </si>
   <si>
@@ -1126,9 +1108,6 @@
     <t>pezas_jotas_jota-de-arbo-1_jota-de-arbo-partitura_2_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_jotas_jota-de-arbo_jota-de-arbo-partitura_2_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_jotas_jota-de-beigondo_jota-de-beigondo-partitura_2_e_1.krn</t>
   </si>
   <si>
@@ -1141,12 +1120,6 @@
     <t>pezas_jotas_jota-de-foxado_jota-de-foxado-partitura_2_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_jotas_jota-de-paradela_jota-de-paradela-partitura_2_e_1.krn</t>
-  </si>
-  <si>
-    <t>pezas_jotas_jota-de-poio_jota-de-poio-partitura_1_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_jotas_jota-de-pontevedra-5_jota-de-pontevedra-partitura_1_e_1.krn</t>
   </si>
   <si>
@@ -1165,9 +1138,6 @@
     <t>pezas_jotas_jota-de-son-1_jota-de-son-partitura_1_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_jotas_jota-de-tui_jota-de-tui-partitura-1_2_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_jotas_jota-de-tui_jota-de-tui-partitura_1_e_1.krn</t>
   </si>
   <si>
@@ -1198,15 +1168,9 @@
     <t>pezas_marchas_batendo-rexo_batendo-rexo-partitura_2_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_marchas_chovendo-en-compostela_chovendo-en-compostela-partitura_2_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_marchas_marcha-2_marcha-partitura_1_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_marchas_marcha-3_marcha-partitura_2_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_marchas_marcha-de-campano_marcha-de-campano-partitura_1_e_1.krn</t>
   </si>
   <si>
@@ -1279,9 +1243,6 @@
     <t>pezas_marchas_o-santino_o-santino-partitura_2_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_marchas_vinte-anos_vinte-anos-partitura_1_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_mazurcas_a-balastreira_a-balastreira-partitura_2_e_1.krn</t>
   </si>
   <si>
@@ -1414,9 +1375,6 @@
     <t>pezas_muineiras_pra-carballo_pra-carballo-partitura_2_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_muineiras_sono-da-papuxa_sono-da-papuxa-partitura_1_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_pasacorredoiras_a-entrada-na-festa_a-entrada-na-festa-partitura_2_e_1.krn</t>
   </si>
   <si>
@@ -1429,15 +1387,9 @@
     <t>pezas_pasacorredoiras_de-xolda_de-xolda-partitura-1_2_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_pasacorredoiras_de-xolda_de-xolda-partitura_1_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_pasacorredoiras_no-corpus-de-pontevedra_no-corpus-de-pontevedra-partitura_1_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_pasacorredoiras_o-rodicio_o-rodicio-partitura_1_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_pasacorredoiras_pasacalles-1_pasacalles-partitura_1_e_1.krn</t>
   </si>
   <si>
@@ -1465,9 +1417,6 @@
     <t>pezas_pasacorredoiras_pasacorredoiras-2_pasacorredoiras-partitura-1_1_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_pasacorredoiras_pasacorredoiras-2_pasacorredoiras-partitura_1_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_pasacorredoiras_pasacorredoiras-5_pasacorredoiras_2_e_1.krn</t>
   </si>
   <si>
@@ -1477,9 +1426,6 @@
     <t>pezas_pasacorredoiras_pasacorredoiras-da-fonsagrada_pasacorredoiras-da-fonsagrada-partitura-1_1_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_pasacorredoiras_pasacorredoiras-da-fonsagrada_pasodoble-da-fonsagrada-partitura_2_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_pasacorredoiras_pasacorredoiras-de-campano_pasacorredoiras-de-campano-partitura_1_e_1.krn</t>
   </si>
   <si>
@@ -1489,9 +1435,6 @@
     <t>pezas_pasacorredoiras_pasacorredoiras-de-ponteareas_pasacorredoiras-de-ponteareas-partitura_1_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_pasacorredoiras_pasacorredoiras-de-ribadavia_danza-de-ribadavia_1_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_pasacorredoiras_pasacorredoiras-de-ribadavia_pasacorredoiras-de-ribadavia-partitura_1_e_1.krn</t>
   </si>
   <si>
@@ -1576,33 +1519,21 @@
     <t>pezas_pasodobles_pasodoble-dos-fosados_pasodoble-dos-fosados-partitura_2_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_pasodobles_pasodoble-dos-tres-roncos_pasodoble-dos-tres-roncos-partitura_2_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_pasodobles_pasodoble-para-chelo_pasodoble-para-chelo-partitura_2_e_1.krn</t>
   </si>
   <si>
     <t>pezas_pasodobles_pasodoble-pico_pasodoble-pico-partitura-1_2_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_pasodobles_pasodoble-pico_pasodoble-pico-partitura_2_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_pasodobles_pasodoble-romantico_pasodoble-romantico-partitura-1_1_e_1.krn</t>
   </si>
   <si>
     <t>pezas_pasodobles_pasodoble_pasodoble-partitura_2_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_pasodobles_pericote_pericote-partitura_1_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_polca_a-gaita-de-melchor_a-gaita-de-melchor-partitura_2_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_polca_falcatruadas_falcatruadas-partitura_2_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_polca_farruquina_farruquina-partitura-1_2_e_1.krn</t>
   </si>
   <si>
@@ -1618,12 +1549,6 @@
     <t>pezas_polca_polca-2_polca-partitura_2_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_polca_polca-4_polca-partitura_1_e_1.krn</t>
-  </si>
-  <si>
-    <t>pezas_polca_polca-5_polca-partitura_1_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_polca_polca-6_polca-partitura_2_e_1.krn</t>
   </si>
   <si>
@@ -1660,12 +1585,6 @@
     <t>pezas_rumbas_rumba-4_rumba-partitura_2_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_rumbas_rumba-5_rumba-partitura_2_e_1.krn</t>
-  </si>
-  <si>
-    <t>pezas_rumbas_rumba-da-buxaina_rumba-da-buxaina-partitura-1_1_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_rumbas_rumba-da-buxaina_rumba-da-buxaina-partitura_1_e_1.krn</t>
   </si>
   <si>
@@ -1729,9 +1648,6 @@
     <t>pezas_rumbas_tocale-la-bocina_tocale-la-bocina-partitura_1_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_rumbas_xaloucos_xaloucos-partitura_2_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_valses_a-beira-do-rio_a-beira-do-rio-partitura_2_e_1.krn</t>
   </si>
   <si>
@@ -1786,9 +1702,6 @@
     <t>pezas_valses_valse-de-arousa_valse-de-arousa-partitura_2_e_1.krn</t>
   </si>
   <si>
-    <t>pezas_valses_valse-de-cecebre_valse-de-cecebre-partitura_1_e_1.krn</t>
-  </si>
-  <si>
     <t>pezas_valses_valse-de-lalin_valse-de-lalin-partitura_1_e_1.krn</t>
   </si>
   <si>
@@ -1835,6 +1748,93 @@
   </si>
   <si>
     <t>march_Old-Rustic-Bridge_1_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_alalas_vento_vento-partitura_1_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_foliadas_a-marinana_a-marinana-partitura_2_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_foliadas_foliada-de-bergantinos_foliada-de-bergantinos-partitura_2_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_foliadas_foliada-de-chantada_foliada-de-chantada-partitura_2_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_foliadas_foliada-de-viascon_foliada-de-viascon-partitura_2_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_jotas_a-barquina_a-barquina-partitura_2_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_jotas_jota-de-barbeito_jota-de-barbeito-partitura_1_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_jotas_jota-de-lugo_jota-de-lugo-partitura_1_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_jotas_jota-de-outeiro_jota-de-outeiro-partitura_1_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_jotas_jota-de-vilarmaior_jota-de-vilarmaior-partitura_1_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_marchas_himno-galego_himno-galego-partitura_1_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_marchas_marcha-de-riotorto_marcha-de-riotorto-partitura_2_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_marchas_marcha-solemne-do-antergo-reino-de-galicia_marcha-solemne-do-antergo-reino-de-galicia-partitura_2_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_muineiras_reviravolta_reviravolta-partitura_1_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_pasacorredoiras_mina-nena_mina-nena-partitura_2_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_pasacorredoiras_os-rueiros_os-rueiros-partitura_2_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_polca_carrasqueira_carrasqueira-partitura_2_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_polca_danza-da-cruz_danza-da-cruz-partitura_2_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_polca_a-pequerrecha_a-pequerrecha-partitura_2_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_valses_valse-de-escornabois_valse-de-escornabois-partitura_1_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_rumbas_rumba-para-a-busca-do-tesouro_rumba-para-a-busca-do-tesouro-partitura_2_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_rumbas_rumba-corrida_rumba-corrida-partitura_1_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_rumbas_o-verdegaio_o-verdegaio-partitura_1_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_pasacorredoiras_pasacorredoiras-4_pasacorredoiras-partitura_1_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_pasacorredoiras_pasacorredoiras-de-arnoia_pasacorredoiras-de-arnoia-partitura_2_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_pasacorredoiras_pasacorredoiras-de-soutelo_pasacorredoiras-de-soutelo-partitura_1_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_pasodobles_pasodoble-dos-coutos_pasodoble-dos-coutos-partitura_1_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_pasodobles_pasodoble-requinteado_pasodoble-requinteado-partitura_1_e_1.krn</t>
+  </si>
+  <si>
+    <t>pezas_pasodobles_pernas-pra-arriba_pernas-pra-arriba-partitura_1_e_1.krn</t>
   </si>
 </sst>
 </file>
@@ -2268,8 +2268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C601"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E105" sqref="E105"/>
+    <sheetView tabSelected="1" topLeftCell="A505" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E521" sqref="E521"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3299,7 +3299,7 @@
         <v>3</v>
       </c>
       <c r="C93" t="s">
-        <v>600</v>
+        <v>571</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
@@ -3310,7 +3310,7 @@
         <v>3</v>
       </c>
       <c r="C94" t="s">
-        <v>601</v>
+        <v>572</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -3420,7 +3420,7 @@
         <v>3</v>
       </c>
       <c r="C104" t="s">
-        <v>602</v>
+        <v>573</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
@@ -3431,7 +3431,7 @@
         <v>3</v>
       </c>
       <c r="C105" t="s">
-        <v>603</v>
+        <v>574</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
@@ -3519,7 +3519,7 @@
         <v>3</v>
       </c>
       <c r="C113" t="s">
-        <v>604</v>
+        <v>575</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
@@ -5917,7 +5917,7 @@
         <v>299</v>
       </c>
       <c r="C331" t="s">
-        <v>329</v>
+        <v>576</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.35">
@@ -5928,7 +5928,7 @@
         <v>299</v>
       </c>
       <c r="C332" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.35">
@@ -5939,7 +5939,7 @@
         <v>299</v>
       </c>
       <c r="C333" t="s">
-        <v>331</v>
+        <v>577</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.35">
@@ -5950,7 +5950,7 @@
         <v>299</v>
       </c>
       <c r="C334" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.35">
@@ -5961,7 +5961,7 @@
         <v>299</v>
       </c>
       <c r="C335" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.35">
@@ -5972,7 +5972,7 @@
         <v>299</v>
       </c>
       <c r="C336" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.35">
@@ -5983,7 +5983,7 @@
         <v>299</v>
       </c>
       <c r="C337" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.35">
@@ -5994,7 +5994,7 @@
         <v>299</v>
       </c>
       <c r="C338" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.35">
@@ -6005,7 +6005,7 @@
         <v>299</v>
       </c>
       <c r="C339" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.35">
@@ -6016,7 +6016,7 @@
         <v>299</v>
       </c>
       <c r="C340" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.35">
@@ -6027,7 +6027,7 @@
         <v>299</v>
       </c>
       <c r="C341" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.35">
@@ -6038,7 +6038,7 @@
         <v>299</v>
       </c>
       <c r="C342" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.35">
@@ -6049,7 +6049,7 @@
         <v>299</v>
       </c>
       <c r="C343" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.35">
@@ -6060,7 +6060,7 @@
         <v>299</v>
       </c>
       <c r="C344" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.35">
@@ -6071,7 +6071,7 @@
         <v>299</v>
       </c>
       <c r="C345" t="s">
-        <v>343</v>
+        <v>578</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.35">
@@ -6082,7 +6082,7 @@
         <v>299</v>
       </c>
       <c r="C346" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.35">
@@ -6093,7 +6093,7 @@
         <v>299</v>
       </c>
       <c r="C347" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.35">
@@ -6104,7 +6104,7 @@
         <v>299</v>
       </c>
       <c r="C348" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.35">
@@ -6115,7 +6115,7 @@
         <v>299</v>
       </c>
       <c r="C349" t="s">
-        <v>347</v>
+        <v>579</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.35">
@@ -6126,7 +6126,7 @@
         <v>299</v>
       </c>
       <c r="C350" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.35">
@@ -6137,7 +6137,7 @@
         <v>299</v>
       </c>
       <c r="C351" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.35">
@@ -6148,7 +6148,7 @@
         <v>299</v>
       </c>
       <c r="C352" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.35">
@@ -6159,7 +6159,7 @@
         <v>299</v>
       </c>
       <c r="C353" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.35">
@@ -6170,7 +6170,7 @@
         <v>299</v>
       </c>
       <c r="C354" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.35">
@@ -6181,7 +6181,7 @@
         <v>299</v>
       </c>
       <c r="C355" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.35">
@@ -6192,7 +6192,7 @@
         <v>299</v>
       </c>
       <c r="C356" t="s">
-        <v>354</v>
+        <v>580</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.35">
@@ -6203,7 +6203,7 @@
         <v>299</v>
       </c>
       <c r="C357" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.35">
@@ -6214,7 +6214,7 @@
         <v>299</v>
       </c>
       <c r="C358" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.35">
@@ -6225,7 +6225,7 @@
         <v>299</v>
       </c>
       <c r="C359" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.35">
@@ -6236,7 +6236,7 @@
         <v>299</v>
       </c>
       <c r="C360" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.35">
@@ -6247,7 +6247,7 @@
         <v>299</v>
       </c>
       <c r="C361" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.35">
@@ -6258,7 +6258,7 @@
         <v>299</v>
       </c>
       <c r="C362" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.35">
@@ -6269,7 +6269,7 @@
         <v>299</v>
       </c>
       <c r="C363" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.35">
@@ -6280,7 +6280,7 @@
         <v>299</v>
       </c>
       <c r="C364" t="s">
-        <v>362</v>
+        <v>581</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.35">
@@ -6291,7 +6291,7 @@
         <v>299</v>
       </c>
       <c r="C365" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.35">
@@ -6302,7 +6302,7 @@
         <v>299</v>
       </c>
       <c r="C366" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.35">
@@ -6313,7 +6313,7 @@
         <v>299</v>
       </c>
       <c r="C367" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.35">
@@ -6324,7 +6324,7 @@
         <v>299</v>
       </c>
       <c r="C368" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.35">
@@ -6335,7 +6335,7 @@
         <v>299</v>
       </c>
       <c r="C369" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.35">
@@ -6346,7 +6346,7 @@
         <v>299</v>
       </c>
       <c r="C370" t="s">
-        <v>368</v>
+        <v>582</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.35">
@@ -6357,7 +6357,7 @@
         <v>299</v>
       </c>
       <c r="C371" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.35">
@@ -6368,7 +6368,7 @@
         <v>299</v>
       </c>
       <c r="C372" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.35">
@@ -6379,7 +6379,7 @@
         <v>299</v>
       </c>
       <c r="C373" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.35">
@@ -6390,7 +6390,7 @@
         <v>299</v>
       </c>
       <c r="C374" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.35">
@@ -6401,7 +6401,7 @@
         <v>299</v>
       </c>
       <c r="C375" t="s">
-        <v>373</v>
+        <v>583</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.35">
@@ -6412,7 +6412,7 @@
         <v>299</v>
       </c>
       <c r="C376" t="s">
-        <v>374</v>
+        <v>584</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.35">
@@ -6423,7 +6423,7 @@
         <v>299</v>
       </c>
       <c r="C377" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.35">
@@ -6434,7 +6434,7 @@
         <v>299</v>
       </c>
       <c r="C378" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.35">
@@ -6445,7 +6445,7 @@
         <v>299</v>
       </c>
       <c r="C379" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.35">
@@ -6456,7 +6456,7 @@
         <v>299</v>
       </c>
       <c r="C380" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.35">
@@ -6467,7 +6467,7 @@
         <v>299</v>
       </c>
       <c r="C381" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.35">
@@ -6478,7 +6478,7 @@
         <v>299</v>
       </c>
       <c r="C382" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.35">
@@ -6489,7 +6489,7 @@
         <v>299</v>
       </c>
       <c r="C383" t="s">
-        <v>381</v>
+        <v>585</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.35">
@@ -6500,7 +6500,7 @@
         <v>299</v>
       </c>
       <c r="C384" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.35">
@@ -6511,7 +6511,7 @@
         <v>299</v>
       </c>
       <c r="C385" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.35">
@@ -6522,7 +6522,7 @@
         <v>299</v>
       </c>
       <c r="C386" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.35">
@@ -6533,7 +6533,7 @@
         <v>299</v>
       </c>
       <c r="C387" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.35">
@@ -6544,7 +6544,7 @@
         <v>299</v>
       </c>
       <c r="C388" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.35">
@@ -6555,7 +6555,7 @@
         <v>299</v>
       </c>
       <c r="C389" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.35">
@@ -6566,7 +6566,7 @@
         <v>299</v>
       </c>
       <c r="C390" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.35">
@@ -6577,7 +6577,7 @@
         <v>299</v>
       </c>
       <c r="C391" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.35">
@@ -6588,7 +6588,7 @@
         <v>299</v>
       </c>
       <c r="C392" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.35">
@@ -6599,7 +6599,7 @@
         <v>299</v>
       </c>
       <c r="C393" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.35">
@@ -6610,7 +6610,7 @@
         <v>299</v>
       </c>
       <c r="C394" t="s">
-        <v>392</v>
+        <v>586</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.35">
@@ -6621,7 +6621,7 @@
         <v>299</v>
       </c>
       <c r="C395" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.35">
@@ -6632,7 +6632,7 @@
         <v>299</v>
       </c>
       <c r="C396" t="s">
-        <v>394</v>
+        <v>587</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.35">
@@ -6643,7 +6643,7 @@
         <v>299</v>
       </c>
       <c r="C397" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.35">
@@ -6654,7 +6654,7 @@
         <v>299</v>
       </c>
       <c r="C398" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.35">
@@ -6665,7 +6665,7 @@
         <v>299</v>
       </c>
       <c r="C399" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.35">
@@ -6676,7 +6676,7 @@
         <v>299</v>
       </c>
       <c r="C400" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.35">
@@ -6687,7 +6687,7 @@
         <v>299</v>
       </c>
       <c r="C401" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.35">
@@ -6698,7 +6698,7 @@
         <v>299</v>
       </c>
       <c r="C402" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.35">
@@ -6709,7 +6709,7 @@
         <v>299</v>
       </c>
       <c r="C403" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.35">
@@ -6720,7 +6720,7 @@
         <v>299</v>
       </c>
       <c r="C404" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.35">
@@ -6731,7 +6731,7 @@
         <v>299</v>
       </c>
       <c r="C405" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.35">
@@ -6742,7 +6742,7 @@
         <v>299</v>
       </c>
       <c r="C406" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.35">
@@ -6753,7 +6753,7 @@
         <v>299</v>
       </c>
       <c r="C407" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.35">
@@ -6764,7 +6764,7 @@
         <v>299</v>
       </c>
       <c r="C408" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.35">
@@ -6775,7 +6775,7 @@
         <v>299</v>
       </c>
       <c r="C409" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.35">
@@ -6786,7 +6786,7 @@
         <v>299</v>
       </c>
       <c r="C410" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.35">
@@ -6797,7 +6797,7 @@
         <v>299</v>
       </c>
       <c r="C411" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.35">
@@ -6808,7 +6808,7 @@
         <v>299</v>
       </c>
       <c r="C412" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.35">
@@ -6819,7 +6819,7 @@
         <v>299</v>
       </c>
       <c r="C413" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.35">
@@ -6830,7 +6830,7 @@
         <v>299</v>
       </c>
       <c r="C414" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.35">
@@ -6841,7 +6841,7 @@
         <v>299</v>
       </c>
       <c r="C415" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.35">
@@ -6852,7 +6852,7 @@
         <v>299</v>
       </c>
       <c r="C416" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.35">
@@ -6863,7 +6863,7 @@
         <v>299</v>
       </c>
       <c r="C417" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.35">
@@ -6874,7 +6874,7 @@
         <v>299</v>
       </c>
       <c r="C418" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.35">
@@ -6885,7 +6885,7 @@
         <v>299</v>
       </c>
       <c r="C419" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.35">
@@ -6896,7 +6896,7 @@
         <v>299</v>
       </c>
       <c r="C420" t="s">
-        <v>418</v>
+        <v>406</v>
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.35">
@@ -6907,7 +6907,7 @@
         <v>299</v>
       </c>
       <c r="C421" t="s">
-        <v>419</v>
+        <v>588</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.35">
@@ -6918,7 +6918,7 @@
         <v>299</v>
       </c>
       <c r="C422" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.35">
@@ -6929,7 +6929,7 @@
         <v>299</v>
       </c>
       <c r="C423" t="s">
-        <v>421</v>
+        <v>408</v>
       </c>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.35">
@@ -6940,7 +6940,7 @@
         <v>299</v>
       </c>
       <c r="C424" t="s">
-        <v>422</v>
+        <v>409</v>
       </c>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.35">
@@ -6951,7 +6951,7 @@
         <v>299</v>
       </c>
       <c r="C425" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.35">
@@ -6962,7 +6962,7 @@
         <v>299</v>
       </c>
       <c r="C426" t="s">
-        <v>424</v>
+        <v>411</v>
       </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.35">
@@ -6973,7 +6973,7 @@
         <v>299</v>
       </c>
       <c r="C427" t="s">
-        <v>425</v>
+        <v>412</v>
       </c>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.35">
@@ -6984,7 +6984,7 @@
         <v>299</v>
       </c>
       <c r="C428" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.35">
@@ -6995,7 +6995,7 @@
         <v>299</v>
       </c>
       <c r="C429" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.35">
@@ -7006,7 +7006,7 @@
         <v>299</v>
       </c>
       <c r="C430" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.35">
@@ -7017,7 +7017,7 @@
         <v>299</v>
       </c>
       <c r="C431" t="s">
-        <v>429</v>
+        <v>416</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.35">
@@ -7028,7 +7028,7 @@
         <v>299</v>
       </c>
       <c r="C432" t="s">
-        <v>430</v>
+        <v>417</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.35">
@@ -7039,7 +7039,7 @@
         <v>299</v>
       </c>
       <c r="C433" t="s">
-        <v>431</v>
+        <v>418</v>
       </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.35">
@@ -7050,7 +7050,7 @@
         <v>299</v>
       </c>
       <c r="C434" t="s">
-        <v>432</v>
+        <v>419</v>
       </c>
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.35">
@@ -7061,7 +7061,7 @@
         <v>299</v>
       </c>
       <c r="C435" t="s">
-        <v>433</v>
+        <v>420</v>
       </c>
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.35">
@@ -7072,7 +7072,7 @@
         <v>299</v>
       </c>
       <c r="C436" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.35">
@@ -7083,7 +7083,7 @@
         <v>299</v>
       </c>
       <c r="C437" t="s">
-        <v>435</v>
+        <v>422</v>
       </c>
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.35">
@@ -7094,7 +7094,7 @@
         <v>299</v>
       </c>
       <c r="C438" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
     </row>
     <row r="439" spans="1:3" x14ac:dyDescent="0.35">
@@ -7105,7 +7105,7 @@
         <v>299</v>
       </c>
       <c r="C439" t="s">
-        <v>437</v>
+        <v>424</v>
       </c>
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.35">
@@ -7116,7 +7116,7 @@
         <v>299</v>
       </c>
       <c r="C440" t="s">
-        <v>438</v>
+        <v>425</v>
       </c>
     </row>
     <row r="441" spans="1:3" x14ac:dyDescent="0.35">
@@ -7127,7 +7127,7 @@
         <v>299</v>
       </c>
       <c r="C441" t="s">
-        <v>439</v>
+        <v>426</v>
       </c>
     </row>
     <row r="442" spans="1:3" x14ac:dyDescent="0.35">
@@ -7138,7 +7138,7 @@
         <v>299</v>
       </c>
       <c r="C442" t="s">
-        <v>440</v>
+        <v>427</v>
       </c>
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.35">
@@ -7149,7 +7149,7 @@
         <v>299</v>
       </c>
       <c r="C443" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.35">
@@ -7160,7 +7160,7 @@
         <v>299</v>
       </c>
       <c r="C444" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
     </row>
     <row r="445" spans="1:3" x14ac:dyDescent="0.35">
@@ -7171,7 +7171,7 @@
         <v>299</v>
       </c>
       <c r="C445" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.35">
@@ -7182,7 +7182,7 @@
         <v>299</v>
       </c>
       <c r="C446" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
     </row>
     <row r="447" spans="1:3" x14ac:dyDescent="0.35">
@@ -7193,7 +7193,7 @@
         <v>299</v>
       </c>
       <c r="C447" t="s">
-        <v>445</v>
+        <v>432</v>
       </c>
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.35">
@@ -7204,7 +7204,7 @@
         <v>299</v>
       </c>
       <c r="C448" t="s">
-        <v>446</v>
+        <v>433</v>
       </c>
     </row>
     <row r="449" spans="1:3" x14ac:dyDescent="0.35">
@@ -7215,7 +7215,7 @@
         <v>299</v>
       </c>
       <c r="C449" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
     </row>
     <row r="450" spans="1:3" x14ac:dyDescent="0.35">
@@ -7226,7 +7226,7 @@
         <v>299</v>
       </c>
       <c r="C450" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
     </row>
     <row r="451" spans="1:3" x14ac:dyDescent="0.35">
@@ -7237,7 +7237,7 @@
         <v>299</v>
       </c>
       <c r="C451" t="s">
-        <v>449</v>
+        <v>436</v>
       </c>
     </row>
     <row r="452" spans="1:3" x14ac:dyDescent="0.35">
@@ -7248,7 +7248,7 @@
         <v>299</v>
       </c>
       <c r="C452" t="s">
-        <v>450</v>
+        <v>437</v>
       </c>
     </row>
     <row r="453" spans="1:3" x14ac:dyDescent="0.35">
@@ -7259,7 +7259,7 @@
         <v>299</v>
       </c>
       <c r="C453" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
     </row>
     <row r="454" spans="1:3" x14ac:dyDescent="0.35">
@@ -7270,7 +7270,7 @@
         <v>299</v>
       </c>
       <c r="C454" t="s">
-        <v>452</v>
+        <v>439</v>
       </c>
     </row>
     <row r="455" spans="1:3" x14ac:dyDescent="0.35">
@@ -7281,7 +7281,7 @@
         <v>299</v>
       </c>
       <c r="C455" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
     </row>
     <row r="456" spans="1:3" x14ac:dyDescent="0.35">
@@ -7292,7 +7292,7 @@
         <v>299</v>
       </c>
       <c r="C456" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
     </row>
     <row r="457" spans="1:3" x14ac:dyDescent="0.35">
@@ -7303,7 +7303,7 @@
         <v>299</v>
       </c>
       <c r="C457" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
     </row>
     <row r="458" spans="1:3" x14ac:dyDescent="0.35">
@@ -7314,7 +7314,7 @@
         <v>299</v>
       </c>
       <c r="C458" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
     </row>
     <row r="459" spans="1:3" x14ac:dyDescent="0.35">
@@ -7325,7 +7325,7 @@
         <v>299</v>
       </c>
       <c r="C459" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
     </row>
     <row r="460" spans="1:3" x14ac:dyDescent="0.35">
@@ -7336,7 +7336,7 @@
         <v>299</v>
       </c>
       <c r="C460" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
     </row>
     <row r="461" spans="1:3" x14ac:dyDescent="0.35">
@@ -7347,7 +7347,7 @@
         <v>299</v>
       </c>
       <c r="C461" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
     </row>
     <row r="462" spans="1:3" x14ac:dyDescent="0.35">
@@ -7358,7 +7358,7 @@
         <v>299</v>
       </c>
       <c r="C462" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
     </row>
     <row r="463" spans="1:3" x14ac:dyDescent="0.35">
@@ -7369,7 +7369,7 @@
         <v>299</v>
       </c>
       <c r="C463" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
     </row>
     <row r="464" spans="1:3" x14ac:dyDescent="0.35">
@@ -7380,7 +7380,7 @@
         <v>299</v>
       </c>
       <c r="C464" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
     </row>
     <row r="465" spans="1:3" x14ac:dyDescent="0.35">
@@ -7391,7 +7391,7 @@
         <v>299</v>
       </c>
       <c r="C465" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
     </row>
     <row r="466" spans="1:3" x14ac:dyDescent="0.35">
@@ -7402,7 +7402,7 @@
         <v>299</v>
       </c>
       <c r="C466" t="s">
-        <v>464</v>
+        <v>589</v>
       </c>
     </row>
     <row r="467" spans="1:3" x14ac:dyDescent="0.35">
@@ -7413,7 +7413,7 @@
         <v>299</v>
       </c>
       <c r="C467" t="s">
-        <v>465</v>
+        <v>451</v>
       </c>
     </row>
     <row r="468" spans="1:3" x14ac:dyDescent="0.35">
@@ -7424,7 +7424,7 @@
         <v>299</v>
       </c>
       <c r="C468" t="s">
-        <v>466</v>
+        <v>452</v>
       </c>
     </row>
     <row r="469" spans="1:3" x14ac:dyDescent="0.35">
@@ -7435,7 +7435,7 @@
         <v>299</v>
       </c>
       <c r="C469" t="s">
-        <v>467</v>
+        <v>453</v>
       </c>
     </row>
     <row r="470" spans="1:3" x14ac:dyDescent="0.35">
@@ -7446,7 +7446,7 @@
         <v>299</v>
       </c>
       <c r="C470" t="s">
-        <v>468</v>
+        <v>454</v>
       </c>
     </row>
     <row r="471" spans="1:3" x14ac:dyDescent="0.35">
@@ -7457,7 +7457,7 @@
         <v>299</v>
       </c>
       <c r="C471" t="s">
-        <v>469</v>
+        <v>590</v>
       </c>
     </row>
     <row r="472" spans="1:3" x14ac:dyDescent="0.35">
@@ -7468,7 +7468,7 @@
         <v>299</v>
       </c>
       <c r="C472" t="s">
-        <v>470</v>
+        <v>455</v>
       </c>
     </row>
     <row r="473" spans="1:3" x14ac:dyDescent="0.35">
@@ -7479,7 +7479,7 @@
         <v>299</v>
       </c>
       <c r="C473" t="s">
-        <v>471</v>
+        <v>591</v>
       </c>
     </row>
     <row r="474" spans="1:3" x14ac:dyDescent="0.35">
@@ -7490,7 +7490,7 @@
         <v>299</v>
       </c>
       <c r="C474" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
     </row>
     <row r="475" spans="1:3" x14ac:dyDescent="0.35">
@@ -7501,7 +7501,7 @@
         <v>299</v>
       </c>
       <c r="C475" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
     </row>
     <row r="476" spans="1:3" x14ac:dyDescent="0.35">
@@ -7512,7 +7512,7 @@
         <v>299</v>
       </c>
       <c r="C476" t="s">
-        <v>474</v>
+        <v>458</v>
       </c>
     </row>
     <row r="477" spans="1:3" x14ac:dyDescent="0.35">
@@ -7523,7 +7523,7 @@
         <v>299</v>
       </c>
       <c r="C477" t="s">
-        <v>475</v>
+        <v>459</v>
       </c>
     </row>
     <row r="478" spans="1:3" x14ac:dyDescent="0.35">
@@ -7534,7 +7534,7 @@
         <v>299</v>
       </c>
       <c r="C478" t="s">
-        <v>476</v>
+        <v>460</v>
       </c>
     </row>
     <row r="479" spans="1:3" x14ac:dyDescent="0.35">
@@ -7545,7 +7545,7 @@
         <v>299</v>
       </c>
       <c r="C479" t="s">
-        <v>477</v>
+        <v>461</v>
       </c>
     </row>
     <row r="480" spans="1:3" x14ac:dyDescent="0.35">
@@ -7556,7 +7556,7 @@
         <v>299</v>
       </c>
       <c r="C480" t="s">
-        <v>478</v>
+        <v>462</v>
       </c>
     </row>
     <row r="481" spans="1:3" x14ac:dyDescent="0.35">
@@ -7567,7 +7567,7 @@
         <v>299</v>
       </c>
       <c r="C481" t="s">
-        <v>479</v>
+        <v>463</v>
       </c>
     </row>
     <row r="482" spans="1:3" x14ac:dyDescent="0.35">
@@ -7578,7 +7578,7 @@
         <v>299</v>
       </c>
       <c r="C482" t="s">
-        <v>480</v>
+        <v>464</v>
       </c>
     </row>
     <row r="483" spans="1:3" x14ac:dyDescent="0.35">
@@ -7589,7 +7589,7 @@
         <v>299</v>
       </c>
       <c r="C483" t="s">
-        <v>481</v>
+        <v>599</v>
       </c>
     </row>
     <row r="484" spans="1:3" x14ac:dyDescent="0.35">
@@ -7600,7 +7600,7 @@
         <v>299</v>
       </c>
       <c r="C484" t="s">
-        <v>482</v>
+        <v>465</v>
       </c>
     </row>
     <row r="485" spans="1:3" x14ac:dyDescent="0.35">
@@ -7611,7 +7611,7 @@
         <v>299</v>
       </c>
       <c r="C485" t="s">
-        <v>483</v>
+        <v>466</v>
       </c>
     </row>
     <row r="486" spans="1:3" x14ac:dyDescent="0.35">
@@ -7622,7 +7622,7 @@
         <v>299</v>
       </c>
       <c r="C486" t="s">
-        <v>484</v>
+        <v>467</v>
       </c>
     </row>
     <row r="487" spans="1:3" x14ac:dyDescent="0.35">
@@ -7633,7 +7633,7 @@
         <v>299</v>
       </c>
       <c r="C487" t="s">
-        <v>485</v>
+        <v>600</v>
       </c>
     </row>
     <row r="488" spans="1:3" x14ac:dyDescent="0.35">
@@ -7644,7 +7644,7 @@
         <v>299</v>
       </c>
       <c r="C488" t="s">
-        <v>486</v>
+        <v>468</v>
       </c>
     </row>
     <row r="489" spans="1:3" x14ac:dyDescent="0.35">
@@ -7655,7 +7655,7 @@
         <v>299</v>
       </c>
       <c r="C489" t="s">
-        <v>487</v>
+        <v>469</v>
       </c>
     </row>
     <row r="490" spans="1:3" x14ac:dyDescent="0.35">
@@ -7666,7 +7666,7 @@
         <v>299</v>
       </c>
       <c r="C490" t="s">
-        <v>488</v>
+        <v>470</v>
       </c>
     </row>
     <row r="491" spans="1:3" x14ac:dyDescent="0.35">
@@ -7677,7 +7677,7 @@
         <v>299</v>
       </c>
       <c r="C491" t="s">
-        <v>489</v>
+        <v>601</v>
       </c>
     </row>
     <row r="492" spans="1:3" x14ac:dyDescent="0.35">
@@ -7688,7 +7688,7 @@
         <v>299</v>
       </c>
       <c r="C492" t="s">
-        <v>490</v>
+        <v>471</v>
       </c>
     </row>
     <row r="493" spans="1:3" x14ac:dyDescent="0.35">
@@ -7699,7 +7699,7 @@
         <v>299</v>
       </c>
       <c r="C493" t="s">
-        <v>491</v>
+        <v>472</v>
       </c>
     </row>
     <row r="494" spans="1:3" x14ac:dyDescent="0.35">
@@ -7710,7 +7710,7 @@
         <v>299</v>
       </c>
       <c r="C494" t="s">
-        <v>492</v>
+        <v>473</v>
       </c>
     </row>
     <row r="495" spans="1:3" x14ac:dyDescent="0.35">
@@ -7721,7 +7721,7 @@
         <v>299</v>
       </c>
       <c r="C495" t="s">
-        <v>493</v>
+        <v>474</v>
       </c>
     </row>
     <row r="496" spans="1:3" x14ac:dyDescent="0.35">
@@ -7732,7 +7732,7 @@
         <v>299</v>
       </c>
       <c r="C496" t="s">
-        <v>494</v>
+        <v>475</v>
       </c>
     </row>
     <row r="497" spans="1:3" x14ac:dyDescent="0.35">
@@ -7743,7 +7743,7 @@
         <v>299</v>
       </c>
       <c r="C497" t="s">
-        <v>495</v>
+        <v>476</v>
       </c>
     </row>
     <row r="498" spans="1:3" x14ac:dyDescent="0.35">
@@ -7754,7 +7754,7 @@
         <v>299</v>
       </c>
       <c r="C498" t="s">
-        <v>496</v>
+        <v>477</v>
       </c>
     </row>
     <row r="499" spans="1:3" x14ac:dyDescent="0.35">
@@ -7765,7 +7765,7 @@
         <v>299</v>
       </c>
       <c r="C499" t="s">
-        <v>497</v>
+        <v>478</v>
       </c>
     </row>
     <row r="500" spans="1:3" x14ac:dyDescent="0.35">
@@ -7776,7 +7776,7 @@
         <v>299</v>
       </c>
       <c r="C500" t="s">
-        <v>498</v>
+        <v>479</v>
       </c>
     </row>
     <row r="501" spans="1:3" x14ac:dyDescent="0.35">
@@ -7787,7 +7787,7 @@
         <v>299</v>
       </c>
       <c r="C501" t="s">
-        <v>499</v>
+        <v>480</v>
       </c>
     </row>
     <row r="502" spans="1:3" x14ac:dyDescent="0.35">
@@ -7798,7 +7798,7 @@
         <v>299</v>
       </c>
       <c r="C502" t="s">
-        <v>500</v>
+        <v>481</v>
       </c>
     </row>
     <row r="503" spans="1:3" x14ac:dyDescent="0.35">
@@ -7809,7 +7809,7 @@
         <v>299</v>
       </c>
       <c r="C503" t="s">
-        <v>501</v>
+        <v>482</v>
       </c>
     </row>
     <row r="504" spans="1:3" x14ac:dyDescent="0.35">
@@ -7820,7 +7820,7 @@
         <v>299</v>
       </c>
       <c r="C504" t="s">
-        <v>502</v>
+        <v>483</v>
       </c>
     </row>
     <row r="505" spans="1:3" x14ac:dyDescent="0.35">
@@ -7831,7 +7831,7 @@
         <v>299</v>
       </c>
       <c r="C505" t="s">
-        <v>503</v>
+        <v>484</v>
       </c>
     </row>
     <row r="506" spans="1:3" x14ac:dyDescent="0.35">
@@ -7842,7 +7842,7 @@
         <v>299</v>
       </c>
       <c r="C506" t="s">
-        <v>504</v>
+        <v>485</v>
       </c>
     </row>
     <row r="507" spans="1:3" x14ac:dyDescent="0.35">
@@ -7853,7 +7853,7 @@
         <v>299</v>
       </c>
       <c r="C507" t="s">
-        <v>505</v>
+        <v>486</v>
       </c>
     </row>
     <row r="508" spans="1:3" x14ac:dyDescent="0.35">
@@ -7864,7 +7864,7 @@
         <v>299</v>
       </c>
       <c r="C508" t="s">
-        <v>506</v>
+        <v>487</v>
       </c>
     </row>
     <row r="509" spans="1:3" x14ac:dyDescent="0.35">
@@ -7875,7 +7875,7 @@
         <v>299</v>
       </c>
       <c r="C509" t="s">
-        <v>507</v>
+        <v>488</v>
       </c>
     </row>
     <row r="510" spans="1:3" x14ac:dyDescent="0.35">
@@ -7886,7 +7886,7 @@
         <v>299</v>
       </c>
       <c r="C510" t="s">
-        <v>508</v>
+        <v>489</v>
       </c>
     </row>
     <row r="511" spans="1:3" x14ac:dyDescent="0.35">
@@ -7897,7 +7897,7 @@
         <v>299</v>
       </c>
       <c r="C511" t="s">
-        <v>509</v>
+        <v>490</v>
       </c>
     </row>
     <row r="512" spans="1:3" x14ac:dyDescent="0.35">
@@ -7908,7 +7908,7 @@
         <v>299</v>
       </c>
       <c r="C512" t="s">
-        <v>510</v>
+        <v>491</v>
       </c>
     </row>
     <row r="513" spans="1:3" x14ac:dyDescent="0.35">
@@ -7919,7 +7919,7 @@
         <v>299</v>
       </c>
       <c r="C513" t="s">
-        <v>511</v>
+        <v>492</v>
       </c>
     </row>
     <row r="514" spans="1:3" x14ac:dyDescent="0.35">
@@ -7930,7 +7930,7 @@
         <v>299</v>
       </c>
       <c r="C514" t="s">
-        <v>512</v>
+        <v>493</v>
       </c>
     </row>
     <row r="515" spans="1:3" x14ac:dyDescent="0.35">
@@ -7941,7 +7941,7 @@
         <v>299</v>
       </c>
       <c r="C515" t="s">
-        <v>513</v>
+        <v>494</v>
       </c>
     </row>
     <row r="516" spans="1:3" x14ac:dyDescent="0.35">
@@ -7952,7 +7952,7 @@
         <v>299</v>
       </c>
       <c r="C516" t="s">
-        <v>514</v>
+        <v>495</v>
       </c>
     </row>
     <row r="517" spans="1:3" x14ac:dyDescent="0.35">
@@ -7963,7 +7963,7 @@
         <v>299</v>
       </c>
       <c r="C517" t="s">
-        <v>515</v>
+        <v>496</v>
       </c>
     </row>
     <row r="518" spans="1:3" x14ac:dyDescent="0.35">
@@ -7974,7 +7974,7 @@
         <v>299</v>
       </c>
       <c r="C518" t="s">
-        <v>516</v>
+        <v>497</v>
       </c>
     </row>
     <row r="519" spans="1:3" x14ac:dyDescent="0.35">
@@ -7985,7 +7985,7 @@
         <v>299</v>
       </c>
       <c r="C519" t="s">
-        <v>517</v>
+        <v>498</v>
       </c>
     </row>
     <row r="520" spans="1:3" x14ac:dyDescent="0.35">
@@ -7996,7 +7996,7 @@
         <v>299</v>
       </c>
       <c r="C520" t="s">
-        <v>518</v>
+        <v>602</v>
       </c>
     </row>
     <row r="521" spans="1:3" x14ac:dyDescent="0.35">
@@ -8007,7 +8007,7 @@
         <v>299</v>
       </c>
       <c r="C521" t="s">
-        <v>519</v>
+        <v>499</v>
       </c>
     </row>
     <row r="522" spans="1:3" x14ac:dyDescent="0.35">
@@ -8018,7 +8018,7 @@
         <v>299</v>
       </c>
       <c r="C522" t="s">
-        <v>520</v>
+        <v>500</v>
       </c>
     </row>
     <row r="523" spans="1:3" x14ac:dyDescent="0.35">
@@ -8029,7 +8029,7 @@
         <v>299</v>
       </c>
       <c r="C523" t="s">
-        <v>521</v>
+        <v>603</v>
       </c>
     </row>
     <row r="524" spans="1:3" x14ac:dyDescent="0.35">
@@ -8040,7 +8040,7 @@
         <v>299</v>
       </c>
       <c r="C524" t="s">
-        <v>522</v>
+        <v>501</v>
       </c>
     </row>
     <row r="525" spans="1:3" x14ac:dyDescent="0.35">
@@ -8051,7 +8051,7 @@
         <v>299</v>
       </c>
       <c r="C525" t="s">
-        <v>523</v>
+        <v>502</v>
       </c>
     </row>
     <row r="526" spans="1:3" x14ac:dyDescent="0.35">
@@ -8062,7 +8062,7 @@
         <v>299</v>
       </c>
       <c r="C526" t="s">
-        <v>524</v>
+        <v>604</v>
       </c>
     </row>
     <row r="527" spans="1:3" x14ac:dyDescent="0.35">
@@ -8073,7 +8073,7 @@
         <v>299</v>
       </c>
       <c r="C527" t="s">
-        <v>525</v>
+        <v>503</v>
       </c>
     </row>
     <row r="528" spans="1:3" x14ac:dyDescent="0.35">
@@ -8084,7 +8084,7 @@
         <v>299</v>
       </c>
       <c r="C528" t="s">
-        <v>526</v>
+        <v>594</v>
       </c>
     </row>
     <row r="529" spans="1:3" x14ac:dyDescent="0.35">
@@ -8095,7 +8095,7 @@
         <v>299</v>
       </c>
       <c r="C529" t="s">
-        <v>527</v>
+        <v>504</v>
       </c>
     </row>
     <row r="530" spans="1:3" x14ac:dyDescent="0.35">
@@ -8106,7 +8106,7 @@
         <v>299</v>
       </c>
       <c r="C530" t="s">
-        <v>528</v>
+        <v>505</v>
       </c>
     </row>
     <row r="531" spans="1:3" x14ac:dyDescent="0.35">
@@ -8117,7 +8117,7 @@
         <v>299</v>
       </c>
       <c r="C531" t="s">
-        <v>529</v>
+        <v>506</v>
       </c>
     </row>
     <row r="532" spans="1:3" x14ac:dyDescent="0.35">
@@ -8128,7 +8128,7 @@
         <v>299</v>
       </c>
       <c r="C532" t="s">
-        <v>530</v>
+        <v>507</v>
       </c>
     </row>
     <row r="533" spans="1:3" x14ac:dyDescent="0.35">
@@ -8139,7 +8139,7 @@
         <v>299</v>
       </c>
       <c r="C533" t="s">
-        <v>531</v>
+        <v>508</v>
       </c>
     </row>
     <row r="534" spans="1:3" x14ac:dyDescent="0.35">
@@ -8150,7 +8150,7 @@
         <v>299</v>
       </c>
       <c r="C534" t="s">
-        <v>532</v>
+        <v>592</v>
       </c>
     </row>
     <row r="535" spans="1:3" x14ac:dyDescent="0.35">
@@ -8161,7 +8161,7 @@
         <v>299</v>
       </c>
       <c r="C535" t="s">
-        <v>533</v>
+        <v>593</v>
       </c>
     </row>
     <row r="536" spans="1:3" x14ac:dyDescent="0.35">
@@ -8172,7 +8172,7 @@
         <v>299</v>
       </c>
       <c r="C536" t="s">
-        <v>534</v>
+        <v>509</v>
       </c>
     </row>
     <row r="537" spans="1:3" x14ac:dyDescent="0.35">
@@ -8183,7 +8183,7 @@
         <v>299</v>
       </c>
       <c r="C537" t="s">
-        <v>535</v>
+        <v>510</v>
       </c>
     </row>
     <row r="538" spans="1:3" x14ac:dyDescent="0.35">
@@ -8194,7 +8194,7 @@
         <v>299</v>
       </c>
       <c r="C538" t="s">
-        <v>536</v>
+        <v>511</v>
       </c>
     </row>
     <row r="539" spans="1:3" x14ac:dyDescent="0.35">
@@ -8205,7 +8205,7 @@
         <v>299</v>
       </c>
       <c r="C539" t="s">
-        <v>537</v>
+        <v>512</v>
       </c>
     </row>
     <row r="540" spans="1:3" x14ac:dyDescent="0.35">
@@ -8216,7 +8216,7 @@
         <v>299</v>
       </c>
       <c r="C540" t="s">
-        <v>538</v>
+        <v>513</v>
       </c>
     </row>
     <row r="541" spans="1:3" x14ac:dyDescent="0.35">
@@ -8227,7 +8227,7 @@
         <v>299</v>
       </c>
       <c r="C541" t="s">
-        <v>539</v>
+        <v>514</v>
       </c>
     </row>
     <row r="542" spans="1:3" x14ac:dyDescent="0.35">
@@ -8238,7 +8238,7 @@
         <v>299</v>
       </c>
       <c r="C542" t="s">
-        <v>540</v>
+        <v>515</v>
       </c>
     </row>
     <row r="543" spans="1:3" x14ac:dyDescent="0.35">
@@ -8249,7 +8249,7 @@
         <v>299</v>
       </c>
       <c r="C543" t="s">
-        <v>541</v>
+        <v>516</v>
       </c>
     </row>
     <row r="544" spans="1:3" x14ac:dyDescent="0.35">
@@ -8260,7 +8260,7 @@
         <v>299</v>
       </c>
       <c r="C544" t="s">
-        <v>542</v>
+        <v>517</v>
       </c>
     </row>
     <row r="545" spans="1:3" x14ac:dyDescent="0.35">
@@ -8271,7 +8271,7 @@
         <v>299</v>
       </c>
       <c r="C545" t="s">
-        <v>543</v>
+        <v>518</v>
       </c>
     </row>
     <row r="546" spans="1:3" x14ac:dyDescent="0.35">
@@ -8282,7 +8282,7 @@
         <v>299</v>
       </c>
       <c r="C546" t="s">
-        <v>544</v>
+        <v>519</v>
       </c>
     </row>
     <row r="547" spans="1:3" x14ac:dyDescent="0.35">
@@ -8293,7 +8293,7 @@
         <v>299</v>
       </c>
       <c r="C547" t="s">
-        <v>545</v>
+        <v>520</v>
       </c>
     </row>
     <row r="548" spans="1:3" x14ac:dyDescent="0.35">
@@ -8304,7 +8304,7 @@
         <v>299</v>
       </c>
       <c r="C548" t="s">
-        <v>546</v>
+        <v>598</v>
       </c>
     </row>
     <row r="549" spans="1:3" x14ac:dyDescent="0.35">
@@ -8315,7 +8315,7 @@
         <v>299</v>
       </c>
       <c r="C549" t="s">
-        <v>547</v>
+        <v>597</v>
       </c>
     </row>
     <row r="550" spans="1:3" x14ac:dyDescent="0.35">
@@ -8326,7 +8326,7 @@
         <v>299</v>
       </c>
       <c r="C550" t="s">
-        <v>548</v>
+        <v>521</v>
       </c>
     </row>
     <row r="551" spans="1:3" x14ac:dyDescent="0.35">
@@ -8337,7 +8337,7 @@
         <v>299</v>
       </c>
       <c r="C551" t="s">
-        <v>549</v>
+        <v>522</v>
       </c>
     </row>
     <row r="552" spans="1:3" x14ac:dyDescent="0.35">
@@ -8348,7 +8348,7 @@
         <v>299</v>
       </c>
       <c r="C552" t="s">
-        <v>550</v>
+        <v>523</v>
       </c>
     </row>
     <row r="553" spans="1:3" x14ac:dyDescent="0.35">
@@ -8359,7 +8359,7 @@
         <v>299</v>
       </c>
       <c r="C553" t="s">
-        <v>551</v>
+        <v>524</v>
       </c>
     </row>
     <row r="554" spans="1:3" x14ac:dyDescent="0.35">
@@ -8370,7 +8370,7 @@
         <v>299</v>
       </c>
       <c r="C554" t="s">
-        <v>552</v>
+        <v>525</v>
       </c>
     </row>
     <row r="555" spans="1:3" x14ac:dyDescent="0.35">
@@ -8381,7 +8381,7 @@
         <v>299</v>
       </c>
       <c r="C555" t="s">
-        <v>553</v>
+        <v>526</v>
       </c>
     </row>
     <row r="556" spans="1:3" x14ac:dyDescent="0.35">
@@ -8392,7 +8392,7 @@
         <v>299</v>
       </c>
       <c r="C556" t="s">
-        <v>554</v>
+        <v>527</v>
       </c>
     </row>
     <row r="557" spans="1:3" x14ac:dyDescent="0.35">
@@ -8403,7 +8403,7 @@
         <v>299</v>
       </c>
       <c r="C557" t="s">
-        <v>555</v>
+        <v>528</v>
       </c>
     </row>
     <row r="558" spans="1:3" x14ac:dyDescent="0.35">
@@ -8414,7 +8414,7 @@
         <v>299</v>
       </c>
       <c r="C558" t="s">
-        <v>556</v>
+        <v>529</v>
       </c>
     </row>
     <row r="559" spans="1:3" x14ac:dyDescent="0.35">
@@ -8425,7 +8425,7 @@
         <v>299</v>
       </c>
       <c r="C559" t="s">
-        <v>557</v>
+        <v>530</v>
       </c>
     </row>
     <row r="560" spans="1:3" x14ac:dyDescent="0.35">
@@ -8436,7 +8436,7 @@
         <v>299</v>
       </c>
       <c r="C560" t="s">
-        <v>558</v>
+        <v>531</v>
       </c>
     </row>
     <row r="561" spans="1:3" x14ac:dyDescent="0.35">
@@ -8447,7 +8447,7 @@
         <v>299</v>
       </c>
       <c r="C561" t="s">
-        <v>559</v>
+        <v>532</v>
       </c>
     </row>
     <row r="562" spans="1:3" x14ac:dyDescent="0.35">
@@ -8458,7 +8458,7 @@
         <v>299</v>
       </c>
       <c r="C562" t="s">
-        <v>560</v>
+        <v>533</v>
       </c>
     </row>
     <row r="563" spans="1:3" x14ac:dyDescent="0.35">
@@ -8469,7 +8469,7 @@
         <v>299</v>
       </c>
       <c r="C563" t="s">
-        <v>561</v>
+        <v>534</v>
       </c>
     </row>
     <row r="564" spans="1:3" x14ac:dyDescent="0.35">
@@ -8480,7 +8480,7 @@
         <v>299</v>
       </c>
       <c r="C564" t="s">
-        <v>562</v>
+        <v>535</v>
       </c>
     </row>
     <row r="565" spans="1:3" x14ac:dyDescent="0.35">
@@ -8491,7 +8491,7 @@
         <v>299</v>
       </c>
       <c r="C565" t="s">
-        <v>563</v>
+        <v>536</v>
       </c>
     </row>
     <row r="566" spans="1:3" x14ac:dyDescent="0.35">
@@ -8502,7 +8502,7 @@
         <v>299</v>
       </c>
       <c r="C566" t="s">
-        <v>564</v>
+        <v>537</v>
       </c>
     </row>
     <row r="567" spans="1:3" x14ac:dyDescent="0.35">
@@ -8513,7 +8513,7 @@
         <v>299</v>
       </c>
       <c r="C567" t="s">
-        <v>565</v>
+        <v>538</v>
       </c>
     </row>
     <row r="568" spans="1:3" x14ac:dyDescent="0.35">
@@ -8524,7 +8524,7 @@
         <v>299</v>
       </c>
       <c r="C568" t="s">
-        <v>566</v>
+        <v>539</v>
       </c>
     </row>
     <row r="569" spans="1:3" x14ac:dyDescent="0.35">
@@ -8535,7 +8535,7 @@
         <v>299</v>
       </c>
       <c r="C569" t="s">
-        <v>567</v>
+        <v>540</v>
       </c>
     </row>
     <row r="570" spans="1:3" x14ac:dyDescent="0.35">
@@ -8546,7 +8546,7 @@
         <v>299</v>
       </c>
       <c r="C570" t="s">
-        <v>568</v>
+        <v>541</v>
       </c>
     </row>
     <row r="571" spans="1:3" x14ac:dyDescent="0.35">
@@ -8557,7 +8557,7 @@
         <v>299</v>
       </c>
       <c r="C571" t="s">
-        <v>569</v>
+        <v>596</v>
       </c>
     </row>
     <row r="572" spans="1:3" x14ac:dyDescent="0.35">
@@ -8568,7 +8568,7 @@
         <v>299</v>
       </c>
       <c r="C572" t="s">
-        <v>570</v>
+        <v>542</v>
       </c>
     </row>
     <row r="573" spans="1:3" x14ac:dyDescent="0.35">
@@ -8579,7 +8579,7 @@
         <v>299</v>
       </c>
       <c r="C573" t="s">
-        <v>571</v>
+        <v>543</v>
       </c>
     </row>
     <row r="574" spans="1:3" x14ac:dyDescent="0.35">
@@ -8590,7 +8590,7 @@
         <v>299</v>
       </c>
       <c r="C574" t="s">
-        <v>572</v>
+        <v>544</v>
       </c>
     </row>
     <row r="575" spans="1:3" x14ac:dyDescent="0.35">
@@ -8601,7 +8601,7 @@
         <v>299</v>
       </c>
       <c r="C575" t="s">
-        <v>573</v>
+        <v>545</v>
       </c>
     </row>
     <row r="576" spans="1:3" x14ac:dyDescent="0.35">
@@ -8612,7 +8612,7 @@
         <v>299</v>
       </c>
       <c r="C576" t="s">
-        <v>574</v>
+        <v>546</v>
       </c>
     </row>
     <row r="577" spans="1:3" x14ac:dyDescent="0.35">
@@ -8623,7 +8623,7 @@
         <v>299</v>
       </c>
       <c r="C577" t="s">
-        <v>575</v>
+        <v>547</v>
       </c>
     </row>
     <row r="578" spans="1:3" x14ac:dyDescent="0.35">
@@ -8634,7 +8634,7 @@
         <v>299</v>
       </c>
       <c r="C578" t="s">
-        <v>576</v>
+        <v>548</v>
       </c>
     </row>
     <row r="579" spans="1:3" x14ac:dyDescent="0.35">
@@ -8645,7 +8645,7 @@
         <v>299</v>
       </c>
       <c r="C579" t="s">
-        <v>577</v>
+        <v>549</v>
       </c>
     </row>
     <row r="580" spans="1:3" x14ac:dyDescent="0.35">
@@ -8656,7 +8656,7 @@
         <v>299</v>
       </c>
       <c r="C580" t="s">
-        <v>578</v>
+        <v>550</v>
       </c>
     </row>
     <row r="581" spans="1:3" x14ac:dyDescent="0.35">
@@ -8667,7 +8667,7 @@
         <v>299</v>
       </c>
       <c r="C581" t="s">
-        <v>579</v>
+        <v>551</v>
       </c>
     </row>
     <row r="582" spans="1:3" x14ac:dyDescent="0.35">
@@ -8678,7 +8678,7 @@
         <v>299</v>
       </c>
       <c r="C582" t="s">
-        <v>580</v>
+        <v>552</v>
       </c>
     </row>
     <row r="583" spans="1:3" x14ac:dyDescent="0.35">
@@ -8689,7 +8689,7 @@
         <v>299</v>
       </c>
       <c r="C583" t="s">
-        <v>581</v>
+        <v>553</v>
       </c>
     </row>
     <row r="584" spans="1:3" x14ac:dyDescent="0.35">
@@ -8700,7 +8700,7 @@
         <v>299</v>
       </c>
       <c r="C584" t="s">
-        <v>582</v>
+        <v>554</v>
       </c>
     </row>
     <row r="585" spans="1:3" x14ac:dyDescent="0.35">
@@ -8711,7 +8711,7 @@
         <v>299</v>
       </c>
       <c r="C585" t="s">
-        <v>583</v>
+        <v>555</v>
       </c>
     </row>
     <row r="586" spans="1:3" x14ac:dyDescent="0.35">
@@ -8722,7 +8722,7 @@
         <v>299</v>
       </c>
       <c r="C586" t="s">
-        <v>584</v>
+        <v>556</v>
       </c>
     </row>
     <row r="587" spans="1:3" x14ac:dyDescent="0.35">
@@ -8733,7 +8733,7 @@
         <v>299</v>
       </c>
       <c r="C587" t="s">
-        <v>585</v>
+        <v>557</v>
       </c>
     </row>
     <row r="588" spans="1:3" x14ac:dyDescent="0.35">
@@ -8744,7 +8744,7 @@
         <v>299</v>
       </c>
       <c r="C588" t="s">
-        <v>586</v>
+        <v>558</v>
       </c>
     </row>
     <row r="589" spans="1:3" x14ac:dyDescent="0.35">
@@ -8755,7 +8755,7 @@
         <v>299</v>
       </c>
       <c r="C589" t="s">
-        <v>587</v>
+        <v>559</v>
       </c>
     </row>
     <row r="590" spans="1:3" x14ac:dyDescent="0.35">
@@ -8766,7 +8766,7 @@
         <v>299</v>
       </c>
       <c r="C590" t="s">
-        <v>588</v>
+        <v>595</v>
       </c>
     </row>
     <row r="591" spans="1:3" x14ac:dyDescent="0.35">
@@ -8777,7 +8777,7 @@
         <v>299</v>
       </c>
       <c r="C591" t="s">
-        <v>589</v>
+        <v>560</v>
       </c>
     </row>
     <row r="592" spans="1:3" x14ac:dyDescent="0.35">
@@ -8788,7 +8788,7 @@
         <v>299</v>
       </c>
       <c r="C592" t="s">
-        <v>590</v>
+        <v>561</v>
       </c>
     </row>
     <row r="593" spans="1:3" x14ac:dyDescent="0.35">
@@ -8799,7 +8799,7 @@
         <v>299</v>
       </c>
       <c r="C593" t="s">
-        <v>591</v>
+        <v>562</v>
       </c>
     </row>
     <row r="594" spans="1:3" x14ac:dyDescent="0.35">
@@ -8810,7 +8810,7 @@
         <v>299</v>
       </c>
       <c r="C594" t="s">
-        <v>592</v>
+        <v>563</v>
       </c>
     </row>
     <row r="595" spans="1:3" x14ac:dyDescent="0.35">
@@ -8821,7 +8821,7 @@
         <v>299</v>
       </c>
       <c r="C595" t="s">
-        <v>593</v>
+        <v>564</v>
       </c>
     </row>
     <row r="596" spans="1:3" x14ac:dyDescent="0.35">
@@ -8832,7 +8832,7 @@
         <v>299</v>
       </c>
       <c r="C596" t="s">
-        <v>594</v>
+        <v>565</v>
       </c>
     </row>
     <row r="597" spans="1:3" x14ac:dyDescent="0.35">
@@ -8843,7 +8843,7 @@
         <v>299</v>
       </c>
       <c r="C597" t="s">
-        <v>595</v>
+        <v>566</v>
       </c>
     </row>
     <row r="598" spans="1:3" x14ac:dyDescent="0.35">
@@ -8854,7 +8854,7 @@
         <v>299</v>
       </c>
       <c r="C598" t="s">
-        <v>596</v>
+        <v>567</v>
       </c>
     </row>
     <row r="599" spans="1:3" x14ac:dyDescent="0.35">
@@ -8865,7 +8865,7 @@
         <v>299</v>
       </c>
       <c r="C599" t="s">
-        <v>597</v>
+        <v>568</v>
       </c>
     </row>
     <row r="600" spans="1:3" x14ac:dyDescent="0.35">
@@ -8876,7 +8876,7 @@
         <v>299</v>
       </c>
       <c r="C600" t="s">
-        <v>598</v>
+        <v>569</v>
       </c>
     </row>
     <row r="601" spans="1:3" x14ac:dyDescent="0.35">
@@ -8887,7 +8887,7 @@
         <v>299</v>
       </c>
       <c r="C601" t="s">
-        <v>599</v>
+        <v>570</v>
       </c>
     </row>
   </sheetData>

</xml_diff>